<commit_message>
Mejorado un poco el excel y faltaba alguna asignatura
</commit_message>
<xml_diff>
--- a/Notas Seguimiento.xlsx
+++ b/Notas Seguimiento.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>ASIGNATURA</t>
   </si>
@@ -56,31 +56,34 @@
     <t>RA7</t>
   </si>
   <si>
-    <t>Sistemas Informáticos M01</t>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Sistemas Informáticos</t>
   </si>
   <si>
     <t>M01</t>
   </si>
   <si>
-    <t>Base de Datos M02</t>
+    <t>Base de Datos</t>
   </si>
   <si>
     <t>M02</t>
   </si>
   <si>
-    <t>Programación M03A</t>
+    <t>Programación</t>
   </si>
   <si>
     <t>M03A</t>
   </si>
   <si>
-    <t>Lenguaje de Marcas M04</t>
+    <t>Lenguaje de Marcas</t>
   </si>
   <si>
     <t>M04</t>
   </si>
   <si>
-    <t>Entornos de Desarrollo M05</t>
+    <t>Entornos de Desarrollo</t>
   </si>
   <si>
     <t>M05</t>
@@ -93,6 +96,9 @@
   </si>
   <si>
     <t>Inglés Profesional</t>
+  </si>
+  <si>
+    <t>Digitalitzacion</t>
   </si>
 </sst>
 </file>
@@ -105,7 +111,7 @@
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +124,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -272,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +328,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF76EFF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF91A4B4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -371,6 +382,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF14D2DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -408,12 +425,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,85 +717,79 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -793,10 +798,10 @@
     <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -805,10 +810,10 @@
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -817,10 +822,10 @@
     <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -829,10 +834,10 @@
     <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -841,17 +846,23 @@
     <xf numFmtId="0" fontId="20" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -877,6 +888,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -884,118 +898,133 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1011,6 +1040,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1068,8 +1106,6 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00A3B1C1"/>
-      <color rgb="0091A4B4"/>
       <color rgb="00FFC451"/>
       <color rgb="00F1A172"/>
       <color rgb="00EF9665"/>
@@ -1078,6 +1114,8 @@
       <color rgb="00FFBC3B"/>
       <color rgb="008CBA6A"/>
       <color rgb="00B186F2"/>
+      <color rgb="0076EFF7"/>
+      <color rgb="0014D2DE"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1346,154 +1384,236 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.4285714285714" style="9" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="31.4285714285714" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="25" customHeight="1" spans="1:10">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="1" customFormat="1" ht="25" customHeight="1" spans="1:13">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="13"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A2" s="13" t="s">
+    <row r="2" s="2" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18">
+        <v>0</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="2">
+        <f>AVERAGE(D2:J2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" s="3" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="23">
         <v>9</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="17"/>
-      <c r="J2" s="48"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="3">
+        <f>AVERAGE(D3:J3)</f>
+        <v>9</v>
+      </c>
+      <c r="M3" s="13"/>
     </row>
-    <row r="3" s="3" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21">
-        <v>9</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="22"/>
-      <c r="J3" s="49"/>
+    <row r="4" s="4" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="28">
+        <v>0</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="4">
+        <f>AVERAGE(D4:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="13"/>
     </row>
-    <row r="4" s="4" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="27"/>
-      <c r="J4" s="50"/>
+    <row r="5" s="5" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="5">
+        <f>AVERAGE(D5:J5)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="13"/>
     </row>
-    <row r="5" s="5" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A5" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="32"/>
-      <c r="J5" s="51"/>
+    <row r="6" s="6" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="38">
+        <v>0</v>
+      </c>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="6">
+        <f>AVERAGE(D6:J6)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="13"/>
     </row>
-    <row r="6" s="6" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A6" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="37"/>
-      <c r="J6" s="52"/>
+    <row r="7" s="7" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A7" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="43">
+        <v>0</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="7">
+        <f>AVERAGE(D7:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="13"/>
     </row>
-    <row r="7" s="7" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A7" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="42"/>
-      <c r="J7" s="53"/>
+    <row r="8" s="8" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A8" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="48">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="8">
+        <f>AVERAGE(D8:J8)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="13"/>
     </row>
-    <row r="8" s="8" customFormat="1" ht="49" customHeight="1" spans="1:10">
-      <c r="A8" s="43" t="s">
+    <row r="9" s="9" customFormat="1" ht="49" customHeight="1" spans="1:13">
+      <c r="A9" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="47"/>
-      <c r="J8" s="54"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="53">
+        <v>0</v>
+      </c>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="55"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="9">
+        <f>AVERAGE(D9:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
automatizacion de cositas del excel
</commit_message>
<xml_diff>
--- a/Notas Seguimiento.xlsx
+++ b/Notas Seguimiento.xlsx
@@ -862,7 +862,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1040,6 +1040,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1384,10 +1387,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1472,7 +1475,7 @@
       <c r="J3" s="57"/>
       <c r="K3" s="13"/>
       <c r="L3" s="3">
-        <f>AVERAGE(D3:J3)</f>
+        <f t="shared" ref="L2:L9" si="0">AVERAGE(D3:J3)</f>
         <v>9</v>
       </c>
       <c r="M3" s="13"/>
@@ -1495,7 +1498,7 @@
       <c r="J4" s="58"/>
       <c r="K4" s="13"/>
       <c r="L4" s="4">
-        <f>AVERAGE(D4:J4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4" s="13"/>
@@ -1518,7 +1521,7 @@
       <c r="J5" s="59"/>
       <c r="K5" s="13"/>
       <c r="L5" s="5">
-        <f>AVERAGE(D5:J5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M5" s="13"/>
@@ -1531,17 +1534,16 @@
         <v>19</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="38">
-        <v>0</v>
-      </c>
+      <c r="D6" s="38"/>
       <c r="E6" s="39"/>
       <c r="F6" s="40"/>
       <c r="G6" s="39"/>
       <c r="H6" s="40"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="60"/>
       <c r="K6" s="13"/>
-      <c r="L6" s="6">
-        <f>AVERAGE(D6:J6)</f>
+      <c r="L6" s="61">
+        <f>D6*0.1+E6*0.2+0.2*F6+0.2*G6+0.1*H6+0.1*J6</f>
         <v>0</v>
       </c>
       <c r="M6" s="13"/>
@@ -1561,10 +1563,10 @@
       <c r="F7" s="45"/>
       <c r="G7" s="44"/>
       <c r="H7" s="45"/>
-      <c r="J7" s="61"/>
+      <c r="J7" s="62"/>
       <c r="K7" s="13"/>
       <c r="L7" s="7">
-        <f>AVERAGE(D7:J7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M7" s="13"/>
@@ -1584,10 +1586,10 @@
       <c r="F8" s="50"/>
       <c r="G8" s="49"/>
       <c r="H8" s="50"/>
-      <c r="J8" s="62"/>
+      <c r="J8" s="63"/>
       <c r="K8" s="13"/>
       <c r="L8" s="8">
-        <f>AVERAGE(D8:J8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M8" s="13"/>
@@ -1607,13 +1609,16 @@
       <c r="F9" s="55"/>
       <c r="G9" s="54"/>
       <c r="H9" s="55"/>
-      <c r="J9" s="63"/>
+      <c r="J9" s="64"/>
       <c r="K9" s="13"/>
       <c r="L9" s="9">
-        <f>AVERAGE(D9:J9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M9" s="13"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correcciones ejercicios llenguatge de marques y ahora a subirlo al classroom
</commit_message>
<xml_diff>
--- a/Notas Seguimiento.xlsx
+++ b/Notas Seguimiento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11850"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
-  <si>
-    <t>ASIGNATURA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+  <si>
+    <t>ASIGNATURA 1º CURSO</t>
   </si>
   <si>
     <t>CÓDIGO</t>
@@ -59,6 +59,9 @@
     <t>Media</t>
   </si>
   <si>
+    <t>Empresa</t>
+  </si>
+  <si>
     <t>Sistemas Informáticos</t>
   </si>
   <si>
@@ -99,6 +102,12 @@
   </si>
   <si>
     <t>Digitalitzacion</t>
+  </si>
+  <si>
+    <t>ASIGNATURA 2º CURSO</t>
+  </si>
+  <si>
+    <t>M03B</t>
   </si>
 </sst>
 </file>
@@ -891,14 +900,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1387,82 +1396,85 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.4285714285714" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="31.4285714285714" style="11" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="25" customHeight="1" spans="1:13">
-      <c r="A1" s="11" t="s">
+    <row r="1" s="1" customFormat="1" ht="25" customHeight="1" spans="1:15">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="10"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="2" s="2" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A2" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="18">
-        <v>0</v>
-      </c>
+      <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
       <c r="H2" s="20"/>
       <c r="J2" s="56"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="2">
+      <c r="K2" s="10"/>
+      <c r="L2" s="2" t="e">
         <f>AVERAGE(D2:J2)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
-    <row r="3" s="3" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="3" s="3" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A3" s="21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="23">
@@ -1473,65 +1485,64 @@
       <c r="G3" s="24"/>
       <c r="H3" s="25"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="13"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="3">
         <f t="shared" ref="L2:L9" si="0">AVERAGE(D3:J3)</f>
         <v>9</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
-    <row r="4" s="4" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="4" s="4" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A4" s="26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="17"/>
-      <c r="D4" s="28">
-        <v>0</v>
-      </c>
+      <c r="D4" s="28"/>
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
       <c r="G4" s="29"/>
       <c r="H4" s="30"/>
       <c r="J4" s="58"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="4">
+      <c r="K4" s="10"/>
+      <c r="L4" s="4" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="O4" s="10"/>
     </row>
-    <row r="5" s="5" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="5" s="5" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A5" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="33">
-        <v>0</v>
-      </c>
+      <c r="D5" s="33"/>
       <c r="E5" s="34"/>
       <c r="F5" s="35"/>
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="J5" s="59"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="5">
+      <c r="K5" s="10"/>
+      <c r="L5" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="O5" s="10"/>
     </row>
-    <row r="6" s="6" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="6" s="6" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A6" s="36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="38"/>
@@ -1539,86 +1550,282 @@
       <c r="F6" s="40"/>
       <c r="G6" s="39"/>
       <c r="H6" s="40"/>
-      <c r="I6" s="6"/>
       <c r="J6" s="60"/>
-      <c r="K6" s="13"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="61">
         <f>D6*0.1+E6*0.2+0.2*F6+0.2*G6+0.1*H6+0.1*J6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="10"/>
+      <c r="O6" s="10"/>
     </row>
-    <row r="7" s="7" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="7" s="7" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A7" s="41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="43">
-        <v>0</v>
-      </c>
+      <c r="D7" s="43"/>
       <c r="E7" s="44"/>
       <c r="F7" s="45"/>
       <c r="G7" s="44"/>
       <c r="H7" s="45"/>
       <c r="J7" s="62"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="7">
+      <c r="K7" s="10"/>
+      <c r="L7" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="O7" s="10"/>
     </row>
-    <row r="8" s="8" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="8" s="8" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="17"/>
-      <c r="D8" s="48">
-        <v>0</v>
-      </c>
+      <c r="D8" s="48"/>
       <c r="E8" s="49"/>
       <c r="F8" s="50"/>
       <c r="G8" s="49"/>
       <c r="H8" s="50"/>
       <c r="J8" s="63"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="8">
+      <c r="K8" s="10"/>
+      <c r="L8" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="O8" s="10"/>
     </row>
-    <row r="9" s="9" customFormat="1" ht="49" customHeight="1" spans="1:13">
+    <row r="9" s="9" customFormat="1" ht="49" customHeight="1" spans="1:15">
       <c r="A9" s="51" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="17"/>
-      <c r="D9" s="53">
-        <v>0</v>
-      </c>
+      <c r="D9" s="53"/>
       <c r="E9" s="54"/>
       <c r="F9" s="55"/>
       <c r="G9" s="54"/>
       <c r="H9" s="55"/>
       <c r="J9" s="64"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="9">
+      <c r="K9" s="10"/>
+      <c r="L9" s="9" t="e">
         <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" s="10" customFormat="1" ht="53" customHeight="1"/>
+    <row r="11" s="1" customFormat="1" ht="25" customHeight="1" spans="1:15">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="10"/>
+      <c r="N11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="2" t="e">
+        <f t="shared" ref="L12:L15" si="1">AVERAGE(D12:J12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="10"/>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" s="3" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" s="4" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" s="5" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" s="6" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="61">
+        <f>D16*0.1+E16*0.2+0.2*F16+0.2*G16+0.1*H16+0.1*J16</f>
         <v>0</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M16" s="10"/>
+      <c r="O16" s="10"/>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12"/>
+    <row r="17" s="7" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A17" s="41"/>
+      <c r="B17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="7" t="e">
+        <f t="shared" ref="L17:L19" si="2">AVERAGE(D17:J17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="10"/>
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" s="8" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A18" s="46"/>
+      <c r="B18" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" s="9" customFormat="1" ht="49" customHeight="1" spans="1:15">
+      <c r="A19" s="51"/>
+      <c r="B19" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="55"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="10"/>
+      <c r="O19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>